<commit_message>
Added backup for report
</commit_message>
<xml_diff>
--- a/LOGREG/LogReg Summary.xlsx
+++ b/LOGREG/LogReg Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nusu-my.sharepoint.com/personal/e0021787_u_nus_edu/Documents/ISS/SA4108/9. CA/00009---ML-Project/LOGREG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive - National University of Singapore\ISS\SA4108\9. CA\00009---ML-Project\LOGREG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{9160D6EB-20C0-4AEF-AC3C-5F154861320C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{735C49A5-84A7-4A4D-88ED-9CE9CEE0A774}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{9160D6EB-20C0-4AEF-AC3C-5F154861320C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{689221F8-B222-4CD8-8EDD-18ED2424A722}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F044F580-A689-4C37-BA5F-E583754BB95E}"/>
   </bookViews>
@@ -43,16 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
-  <si>
-    <t>Duration of Model</t>
-  </si>
-  <si>
-    <t>Accuracy Score of Train Model</t>
-  </si>
-  <si>
-    <t>Accuracy Score of Test  Model</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>X_train columns</t>
   </si>
@@ -140,11 +131,26 @@
   <si>
     <t>Model 3 with no PCA</t>
   </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Duration of Model (seconds)</t>
+  </si>
+  <si>
+    <t>Accuracy Score of Train Model (Max = 1.0)</t>
+  </si>
+  <si>
+    <t>Accuracy Score of Test  Model (Max = 1.0)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,19 +186,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -222,6 +259,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Duration of Logistic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Regression</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Model</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -267,7 +337,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Duration of Model</c:v>
+                  <c:v>Duration of Model (seconds)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -324,10 +394,10 @@
             <c:numRef>
               <c:f>Sheet2!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.22639584541320801</c:v>
+                  <c:v>8.5770368576049805E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.09705924987792E-2</c:v>
@@ -339,7 +409,7 @@
                   <c:v>1.4959573745727499E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.5770368576049805E-2</c:v>
+                  <c:v>0.22639584541320801</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.20644807815551758</c:v>
@@ -385,6 +455,34 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -450,7 +548,21 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -572,7 +684,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Accuracy of</a:t>
+              <a:t>Accuracy of Logistic Regression</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -627,7 +739,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Accuracy Score of Train Model</c:v>
+                  <c:v>Accuracy Score of Train Model (Max = 1.0)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -684,10 +796,10 @@
             <c:numRef>
               <c:f>Sheet2!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.46998020672971103</c:v>
+                  <c:v>0.98130635583901404</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.97932702881020395</c:v>
@@ -699,7 +811,7 @@
                   <c:v>0.98636463602375102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98130635583901404</c:v>
+                  <c:v>0.46998020672971103</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.48251594457884317</c:v>
@@ -734,7 +846,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Accuracy Score of Test  Model</c:v>
+                  <c:v>Accuracy Score of Test  Model (Max = 1.0)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -791,10 +903,10 @@
             <c:numRef>
               <c:f>Sheet2!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.45692307692307599</c:v>
+                  <c:v>0.97230769230769198</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.97230769230769198</c:v>
@@ -806,7 +918,7 @@
                   <c:v>0.98256410256410198</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97230769230769198</c:v>
+                  <c:v>0.45692307692307599</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.46820512820512822</c:v>
@@ -852,6 +964,34 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -917,7 +1057,21 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2131,8 +2285,8 @@
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3600450</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -2167,8 +2321,8 @@
       <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3571875</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
@@ -2222,13 +2376,13 @@
     <sortCondition ref="A1:A11"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{09FA7A10-78C1-490D-90E1-9EEB60F70D7E}" uniqueName="1" name="Model Name" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{75E95EC7-6203-4BDD-94F5-610081F9A02F}" uniqueName="2" name="Duration of Model" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{4EF2CABC-E2EA-47D9-AB3E-20A63222F2CE}" uniqueName="3" name="Accuracy Score of Train Model" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{8E2E2E9F-916A-49A8-9972-4E04EAA7F692}" uniqueName="4" name="Accuracy Score of Test  Model" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{21A73E3E-5802-41A7-A536-4BB309A3AB36}" uniqueName="5" name="X_train columns" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{9E10B0D3-E371-4606-A758-29C3D5E0B581}" uniqueName="6" name="Y_train columns" queryTableFieldId="6" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{B16B7C5B-391C-4CEC-BE09-18F8CE6450D3}" uniqueName="7" name="PCA" queryTableFieldId="7"/>
+    <tableColumn id="1" xr3:uid="{09FA7A10-78C1-490D-90E1-9EEB60F70D7E}" uniqueName="1" name="Model Name" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{75E95EC7-6203-4BDD-94F5-610081F9A02F}" uniqueName="2" name="Duration of Model (seconds)" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4EF2CABC-E2EA-47D9-AB3E-20A63222F2CE}" uniqueName="3" name="Accuracy Score of Train Model (Max = 1.0)" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8E2E2E9F-916A-49A8-9972-4E04EAA7F692}" uniqueName="4" name="Accuracy Score of Test  Model (Max = 1.0)" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{21A73E3E-5802-41A7-A536-4BB309A3AB36}" uniqueName="5" name="X_train columns" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{9E10B0D3-E371-4606-A758-29C3D5E0B581}" uniqueName="6" name="Y_train columns" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{B16B7C5B-391C-4CEC-BE09-18F8CE6450D3}" uniqueName="7" name="PCA" queryTableFieldId="7" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{C84D5715-B9E9-49F9-A251-7503A14E17D6}" uniqueName="8" name="Remarks" queryTableFieldId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2534,297 +2688,305 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2549AE13-12E9-4A2C-845E-9422587AF352}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="24.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4">
+        <v>8.5770368576049805E-2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.98130635583901404</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.97230769230769198</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2">
-        <v>0.22639584541320801</v>
-      </c>
-      <c r="C2">
-        <v>0.46998020672971103</v>
-      </c>
-      <c r="D2">
-        <v>0.45692307692307599</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4">
         <v>1.09705924987792E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.97932702881020395</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.97230769230769198</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3">
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4">
         <v>7.9791545867919905E-3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.98614471079832799</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.98358974358974305</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4">
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4">
         <v>1.4959573745727499E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.98636463602375102</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.98256410256410198</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6">
-        <v>8.5770368576049805E-2</v>
-      </c>
-      <c r="C6">
-        <v>0.98130635583901404</v>
-      </c>
-      <c r="D6">
-        <v>0.97230769230769198</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.22639584541320801</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.46998020672971103</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.45692307692307599</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4">
         <v>0.20644807815551758</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>0.48251594457884317</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.46820512820512822</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7">
+      <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4">
         <v>0.140623569488525</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>0.93072355399164197</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>0.93384615384615299</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4">
         <v>2.15270519256591E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>0.93072355399164197</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>0.93384615384615299</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4">
         <v>2.2939920425415001E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>0.93072355399164197</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>0.93384615384615299</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4">
         <v>2.8923511505126901E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>0.93072355399164197</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>0.93384615384615299</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2853,6 +3015,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F9A9D329B328C4BBE0DFCEE619434D8" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="621097ee10fcdee7bb50f608133aa18a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0dc3e94b-94e4-4e05-983e-659540d929e0" xmlns:ns4="d0dea29b-97e7-479c-b803-7fedf1230a1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="569fcded7e487b9f530543b5d130afe3" ns3:_="" ns4:_="">
     <xsd:import namespace="0dc3e94b-94e4-4e05-983e-659540d929e0"/>
@@ -3075,21 +3252,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{952CB676-7A77-4C55-A184-830C940E6127}">
   <ds:schemaRefs>
@@ -3099,6 +3261,31 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10055DB7-A2D6-48D3-9475-9F145CD3302F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d0dea29b-97e7-479c-b803-7fedf1230a1e"/>
+    <ds:schemaRef ds:uri="0dc3e94b-94e4-4e05-983e-659540d929e0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2492DE-59AE-433B-B7B9-3C855ADFEF66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21D5F726-7B12-4DB6-AE46-3D36D3EAF0B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3115,29 +3302,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2492DE-59AE-433B-B7B9-3C855ADFEF66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10055DB7-A2D6-48D3-9475-9F145CD3302F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0dc3e94b-94e4-4e05-983e-659540d929e0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d0dea29b-97e7-479c-b803-7fedf1230a1e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>